<commit_message>
Error del output y función para c_star.
</commit_message>
<xml_diff>
--- a/Input.xlsx
+++ b/Input.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="37">
   <si>
     <t xml:space="preserve">Etiqueta</t>
   </si>
@@ -56,6 +56,12 @@
     <t xml:space="preserve">CDOM443_factor</t>
   </si>
   <si>
+    <t xml:space="preserve">A_c_star_660</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E_c_star_660</t>
+  </si>
+  <si>
     <t xml:space="preserve">Astar_NAP_443</t>
   </si>
   <si>
@@ -104,10 +110,22 @@
     <t xml:space="preserve">0, 5</t>
   </si>
   <si>
+    <t xml:space="preserve">Voss92: 0.314</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Voss92: 0.57</t>
+  </si>
+  <si>
     <t xml:space="preserve">valores posibles: 0, 10, …, 90</t>
   </si>
   <si>
     <t xml:space="preserve">valores posibles: 0, 90, 135, 180</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Morel02: 0.407</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Morel02: 0.795</t>
   </si>
   <si>
     <t xml:space="preserve">Si CHL_steps es un único número, el programa lo interpreta como la cantidad de pasos entre el valor máximo y el mínimo. Lo mismo con NAP_steps y CDOM_steps.</t>
@@ -123,7 +141,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -151,6 +169,11 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="6">
@@ -219,7 +242,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -244,7 +267,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -325,28 +356,29 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:X3"/>
+  <dimension ref="A1:Z4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K3" activeCellId="0" sqref="K3"/>
+      <selection pane="topLeft" activeCell="L2" activeCellId="0" sqref="L2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.13671875" defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.15625" defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="13.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="13.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="14.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="14.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="7.56"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="15.44"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="11.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="18.77"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="18.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="15.56"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="16.56"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="0" width="25.74"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="0" width="27.84"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="13.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="13" style="0" width="14.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="14.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="7.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="15.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="11.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="18.77"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="18.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="15.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="0" width="16.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="25" style="0" width="25.74"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="26" style="0" width="27.84"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -383,10 +415,10 @@
       <c r="K1" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="L1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="4" t="s">
+      <c r="M1" s="6" t="s">
         <v>12</v>
       </c>
       <c r="N1" s="4" t="s">
@@ -395,115 +427,141 @@
       <c r="O1" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="5" t="s">
+      <c r="P1" s="4" t="s">
         <v>15</v>
       </c>
       <c r="Q1" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="3" t="s">
+      <c r="R1" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="0" t="s">
+      <c r="S1" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="6" t="s">
+      <c r="T1" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="6" t="s">
+      <c r="U1" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="0" t="s">
+      <c r="V1" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="6" t="s">
+      <c r="W1" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="6" t="s">
+      <c r="X1" s="0" t="s">
         <v>23</v>
+      </c>
+      <c r="Y1" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="Z1" s="7" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="C2" s="6" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="D2" s="6" t="n">
+        <v>27</v>
+      </c>
+      <c r="C2" s="7" t="n">
+        <v>5</v>
+      </c>
+      <c r="D2" s="7" t="n">
         <v>10</v>
       </c>
-      <c r="E2" s="0" t="n">
-        <v>1.5</v>
-      </c>
-      <c r="F2" s="6" t="n">
+      <c r="E2" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="F2" s="7" t="n">
+        <v>40</v>
+      </c>
+      <c r="G2" s="7" t="n">
+        <v>50</v>
+      </c>
+      <c r="H2" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="I2" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="J2" s="7" t="n">
         <v>10</v>
       </c>
-      <c r="G2" s="6" t="n">
-        <v>50</v>
-      </c>
-      <c r="H2" s="6" t="n">
-        <v>1.5</v>
-      </c>
-      <c r="I2" s="6" t="n">
-        <v>1</v>
-      </c>
-      <c r="J2" s="6" t="n">
-        <v>10</v>
-      </c>
-      <c r="K2" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="L2" s="6" t="n">
+      <c r="K2" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="L2" s="7" t="n">
+        <v>0.314</v>
+      </c>
+      <c r="M2" s="7" t="n">
+        <v>0.57</v>
+      </c>
+      <c r="N2" s="7" t="n">
         <v>0.041</v>
       </c>
-      <c r="M2" s="6" t="n">
+      <c r="O2" s="7" t="n">
         <v>0.55</v>
       </c>
-      <c r="N2" s="6" t="n">
+      <c r="P2" s="7" t="n">
         <v>-0.0123</v>
       </c>
-      <c r="O2" s="6" t="n">
+      <c r="Q2" s="7" t="n">
         <v>-0.3749</v>
       </c>
-      <c r="P2" s="6" t="n">
+      <c r="R2" s="7" t="n">
         <v>-0.0149</v>
       </c>
-      <c r="Q2" s="6" t="n">
+      <c r="S2" s="7" t="n">
         <v>0.018</v>
       </c>
-      <c r="R2" s="0" t="n">
+      <c r="T2" s="0" t="n">
         <v>0.006</v>
       </c>
-      <c r="S2" s="0" t="n">
+      <c r="U2" s="0" t="n">
         <v>40</v>
       </c>
-      <c r="T2" s="0" t="n">
+      <c r="V2" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="U2" s="0" t="n">
+      <c r="W2" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="V2" s="0" t="n">
+      <c r="X2" s="0" t="n">
         <v>5</v>
       </c>
-      <c r="W2" s="6" t="n">
+      <c r="Y2" s="7" t="n">
         <v>40</v>
       </c>
-      <c r="X2" s="6" t="n">
+      <c r="Z2" s="7" t="n">
         <v>135</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="K3" s="6"/>
-      <c r="W3" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="X3" s="6" t="s">
-        <v>28</v>
+      <c r="K3" s="7"/>
+      <c r="L3" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="M3" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="Y3" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="Z3" s="7" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L4" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="M4" s="8" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -528,16 +586,16 @@
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.9140625" defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.9296875" defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Combinatorio para el bloque de simulaciones.
</commit_message>
<xml_diff>
--- a/Input.xlsx
+++ b/Input.xlsx
@@ -104,7 +104,7 @@
     <t xml:space="preserve">phi_view</t>
   </si>
   <si>
-    <t xml:space="preserve">PRUEBA</t>
+    <t xml:space="preserve">A</t>
   </si>
   <si>
     <t xml:space="preserve">prueba</t>
@@ -351,18 +351,18 @@
   </sheetPr>
   <dimension ref="A1:AA4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="R1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="W2" activeCellId="0" sqref="W2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.19140625" defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.2109375" defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="13.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="13.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="13.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="13" style="0" width="14.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="19.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="19.19"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="1" width="14.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="7.56"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="15.44"/>
@@ -586,7 +586,7 @@
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.95703125" defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.9765625" defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">

</xml_diff>

<commit_message>
Agregué 'Graficar_HL' y arreglé la lectura de la tabla.
</commit_message>
<xml_diff>
--- a/Input.xlsx
+++ b/Input.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
   <si>
     <t xml:space="preserve">Etiqueta</t>
   </si>
@@ -104,16 +104,19 @@
     <t xml:space="preserve">phi_view</t>
   </si>
   <si>
-    <t xml:space="preserve">A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">prueba</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0, 5</t>
+    <t xml:space="preserve">v8-no_fl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Versión 8 SIN FLUORESCENCIA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0, 0.1, 1.0, 5.0, 10.0</t>
   </si>
   <si>
     <t xml:space="preserve">0, 0.004, 0.008, 0.012</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.01, 0.018, 0.03</t>
   </si>
   <si>
     <t xml:space="preserve">Voss92: 0.314</t>
@@ -351,11 +354,11 @@
   </sheetPr>
   <dimension ref="A1:AA4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="J1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="T2" activeCellId="0" sqref="T2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.2109375" defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.2265625" defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="13.33"/>
@@ -466,22 +469,22 @@
         <v>28</v>
       </c>
       <c r="C2" s="6" t="n">
-        <v>5</v>
+        <v>0.5</v>
       </c>
       <c r="D2" s="6" t="n">
+        <v>100</v>
+      </c>
+      <c r="E2" s="0" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="F2" s="6" t="n">
         <v>10</v>
       </c>
-      <c r="E2" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="F2" s="6" t="n">
-        <v>40</v>
-      </c>
       <c r="G2" s="6" t="n">
-        <v>50</v>
-      </c>
-      <c r="H2" s="6" t="s">
-        <v>29</v>
+        <v>500</v>
+      </c>
+      <c r="H2" s="6" t="n">
+        <v>1.5</v>
       </c>
       <c r="I2" s="6" t="n">
         <v>1</v>
@@ -516,8 +519,8 @@
       <c r="S2" s="6" t="n">
         <v>-0.0149</v>
       </c>
-      <c r="T2" s="6" t="n">
-        <v>0.018</v>
+      <c r="T2" s="6" t="s">
+        <v>31</v>
       </c>
       <c r="U2" s="0" t="n">
         <v>0.006</v>
@@ -544,24 +547,24 @@
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="K3" s="6"/>
       <c r="L3" s="6" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="M3" s="6" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="Z3" s="6" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="AA3" s="6" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="L4" s="6" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="M4" s="6" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -586,16 +589,16 @@
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.9765625" defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.9921875" defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Flag para el output.
</commit_message>
<xml_diff>
--- a/Input.xlsx
+++ b/Input.xlsx
@@ -374,7 +374,7 @@
       <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.23828125" defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.25390625" defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="13.33"/>
@@ -494,7 +494,7 @@
         <v>0</v>
       </c>
       <c r="D2" s="0" t="n">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="E2" s="7" t="n">
         <v>0.5</v>
@@ -617,7 +617,7 @@
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.00390625" defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.01953125" defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">

</xml_diff>

<commit_message>
Chequeo de directorios de HL y HE60.
</commit_message>
<xml_diff>
--- a/Input.xlsx
+++ b/Input.xlsx
@@ -374,7 +374,7 @@
       <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.2890625" defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.30859375" defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="13.33"/>
@@ -491,10 +491,10 @@
         <v>30</v>
       </c>
       <c r="C2" s="0" t="n">
-        <v>120</v>
+        <v>130</v>
       </c>
       <c r="D2" s="0" t="n">
-        <v>130</v>
+        <v>150</v>
       </c>
       <c r="E2" s="7" t="n">
         <v>0.5</v>
@@ -617,7 +617,7 @@
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.0546875" defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.07421875" defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">

</xml_diff>

<commit_message>
Gráficos para combinaciones de ángulos.
</commit_message>
<xml_diff>
--- a/Input.xlsx
+++ b/Input.xlsx
@@ -371,10 +371,10 @@
   <dimension ref="A1:AC4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
+      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.42578125" defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.47265625" defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="13.33"/>
@@ -491,10 +491,10 @@
         <v>30</v>
       </c>
       <c r="C2" s="0" t="n">
-        <v>460</v>
+        <v>547</v>
       </c>
       <c r="D2" s="0" t="n">
-        <v>465</v>
+        <v>550</v>
       </c>
       <c r="E2" s="7" t="n">
         <v>0.5</v>
@@ -617,7 +617,7 @@
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.19140625" defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.23828125" defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">

</xml_diff>

<commit_message>
Fluorescencia en el input y carpetas para P&D.
</commit_message>
<xml_diff>
--- a/Input.xlsx
+++ b/Input.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
   <si>
     <t xml:space="preserve">Etiqueta</t>
   </si>
@@ -62,10 +62,10 @@
     <t xml:space="preserve">CDOM443_factor</t>
   </si>
   <si>
-    <t xml:space="preserve">A_c_star_660</t>
-  </si>
-  <si>
-    <t xml:space="preserve">E_c_star_660</t>
+    <t xml:space="preserve">A_c_phy_star_660</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E_c_phy_star_660</t>
   </si>
   <si>
     <t xml:space="preserve">Astar_NAP_443</t>
@@ -110,7 +110,13 @@
     <t xml:space="preserve">phi_view</t>
   </si>
   <si>
-    <t xml:space="preserve">TEST</t>
+    <t xml:space="preserve">fluorescence</t>
+  </si>
+  <si>
+    <t xml:space="preserve">v8_no_fl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Versión 8 – sin fluorescencia</t>
   </si>
   <si>
     <t xml:space="preserve">0, 0.1, 1.0, 5.0, 10.0</t>
@@ -132,6 +138,9 @@
   </si>
   <si>
     <t xml:space="preserve">valores posibles: 0, 90, 135, 180</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0: sin, 1: con</t>
   </si>
   <si>
     <t xml:space="preserve">Morel02: 0.407</t>
@@ -365,19 +374,20 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AC4"/>
+  <dimension ref="A1:AD4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="I7" activeCellId="0" sqref="I7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.578125" defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.60546875" defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="24.78"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="13.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="13.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="13.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="15" style="0" width="14.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="17.96"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="14" style="0" width="16.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="14.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="19.19"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="1" width="14.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="7.56"/>
@@ -479,10 +489,22 @@
       <c r="AC1" s="7" t="s">
         <v>28</v>
       </c>
+      <c r="AD1" s="0" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2" s="0" t="n">
+        <v>6000</v>
+      </c>
+      <c r="D2" s="0" t="n">
+        <v>8000</v>
       </c>
       <c r="E2" s="7" t="n">
         <v>0.5</v>
@@ -509,7 +531,7 @@
         <v>10</v>
       </c>
       <c r="M2" s="7" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="N2" s="7" t="n">
         <v>0.314</v>
@@ -521,7 +543,7 @@
         <v>0.041</v>
       </c>
       <c r="Q2" s="7" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="R2" s="7" t="n">
         <v>0.55</v>
@@ -536,7 +558,7 @@
         <v>-0.0149</v>
       </c>
       <c r="V2" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="W2" s="0" t="n">
         <v>0.006</v>
@@ -558,29 +580,35 @@
       </c>
       <c r="AC2" s="7" t="n">
         <v>135</v>
+      </c>
+      <c r="AD2" s="0" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M3" s="7"/>
       <c r="N3" s="7" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="O3" s="7" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="AB3" s="7" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="AC3" s="7" t="s">
-        <v>36</v>
+        <v>38</v>
+      </c>
+      <c r="AD3" s="0" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="N4" s="7" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="O4" s="7" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -605,16 +633,16 @@
       <selection pane="topLeft" activeCell="K19" activeCellId="0" sqref="K19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.3359375" defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.37109375" defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Corregido el bug: CDOM <-> NAP
</commit_message>
<xml_diff>
--- a/Input.xlsx
+++ b/Input.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
   <si>
     <t xml:space="preserve">Etiqueta</t>
   </si>
@@ -116,13 +116,19 @@
     <t xml:space="preserve">fluorescence</t>
   </si>
   <si>
-    <t xml:space="preserve">TEST_2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Probando Id_start</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0, 1</t>
+    <t xml:space="preserve">v8_no_fl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Versión 8 – sin fluorescencia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0, 0.1, 1.0, 5.0, 10.0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0, 0.004, 0.008, 0.012</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.01, 0.018, 0.03</t>
   </si>
   <si>
     <t xml:space="preserve">Voss92: 0.314</t>
@@ -387,7 +393,7 @@
       <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.66015625" defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.73046875" defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="24.8"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="13.33"/>
@@ -511,13 +517,13 @@
         <v>32</v>
       </c>
       <c r="C2" s="0" t="n">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="D2" s="0" t="n">
-        <v>1000</v>
+        <v>3000</v>
       </c>
       <c r="E2" s="0" t="n">
-        <v>1001</v>
+        <v>4000</v>
       </c>
       <c r="F2" s="8" t="n">
         <v>0.5</v>
@@ -555,8 +561,8 @@
       <c r="Q2" s="8" t="n">
         <v>0.041</v>
       </c>
-      <c r="R2" s="8" t="n">
-        <v>0</v>
+      <c r="R2" s="8" t="s">
+        <v>34</v>
       </c>
       <c r="S2" s="8" t="n">
         <v>0.55</v>
@@ -570,8 +576,8 @@
       <c r="V2" s="8" t="n">
         <v>-0.0149</v>
       </c>
-      <c r="W2" s="8" t="n">
-        <v>0.2</v>
+      <c r="W2" s="8" t="s">
+        <v>35</v>
       </c>
       <c r="X2" s="0" t="n">
         <v>0.006</v>
@@ -601,27 +607,27 @@
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="N3" s="8"/>
       <c r="O3" s="8" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="P3" s="8" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="AC3" s="8" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="AD3" s="8" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="AE3" s="0" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="O4" s="8" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="P4" s="8" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -646,16 +652,16 @@
       <selection pane="topLeft" activeCell="K19" activeCellId="0" sqref="K19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.42578125" defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.48828125" defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>